<commit_message>
cleaned up and fixed some minor errors. Additionally, added some expected failure options
</commit_message>
<xml_diff>
--- a/tests/040_simple_valid.xlsx
+++ b/tests/040_simple_valid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\PycharmProjects\VocExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\PycharmProjects\VocExcel\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8738A27A-2C2D-4772-9519-9D9339E2842A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C24E6F-6AA9-4933-A61B-6325236227F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="13875" yWindow="3015" windowWidth="18390" windowHeight="13335" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17430" yWindow="3585" windowWidth="18390" windowHeight="13335" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>Surround Australia Pty Ltd</t>
   </si>
@@ -1255,9 +1255,6 @@
  http://resource.geosciml.org/classifier/cgi/particletype/xenocryst</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 6, 7</t>
-  </si>
-  <si>
     <t>NADM SLTTs 2004</t>
   </si>
 </sst>
@@ -18426,7 +18423,7 @@
   </sheetPr>
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -18547,7 +18544,7 @@
         <v>72</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="15"/>
     </row>
@@ -18612,7 +18609,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="15"/>
     </row>
@@ -29576,8 +29573,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29665,9 +29662,7 @@
         <v>http://resource.geosciml.org/classifier/cgi/particletype/biogenic_particle</v>
       </c>
       <c r="B3" s="26"/>
-      <c r="C3" s="25" t="s">
-        <v>94</v>
-      </c>
+      <c r="C3" s="25"/>
       <c r="D3" s="24"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>

</xml_diff>